<commit_message>
Modified the graph to show comparison by CRUD operation. This explains the RU comparison more clearly compared to the previous graph.
</commit_message>
<xml_diff>
--- a/output/analysis/session_consistency_06212020/Async CRUD Ops.xlsx
+++ b/output/analysis/session_consistency_06212020/Async CRUD Ops.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/deepu/projects/CosmosSQLCalipers/output/analysis/session_consistency_06212020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C79601A-DA6C-CA40-91BB-4B7DC641E07D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D633C8F-5409-FD4C-A774-68747B2CE992}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{EAD0F799-C2DA-4B48-B443-1B75B3FC14E9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19540" xr2:uid="{EAD0F799-C2DA-4B48-B443-1B75B3FC14E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$29</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$2:$C$29</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
   <si>
     <t>payload</t>
   </si>
@@ -158,6 +153,48 @@
   </si>
   <si>
     <t>async_upsert_400k</t>
+  </si>
+  <si>
+    <t>write_1k</t>
+  </si>
+  <si>
+    <t>write_5k</t>
+  </si>
+  <si>
+    <t>operation</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>5k</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>50k</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>200k</t>
+  </si>
+  <si>
+    <t>400k</t>
+  </si>
+  <si>
+    <t>write</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>replace</t>
+  </si>
+  <si>
+    <t>upsert</t>
   </si>
 </sst>
 </file>
@@ -3113,6 +3150,652 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" baseline="0"/>
+              <a:t>RU consumption by CRUD operation </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>comparison</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="2000" b="1" baseline="0"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>write</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$S$1:$Y$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1k</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5k</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10k</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50k</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100k</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200k</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$S$2:$Y$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>186</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-447B-F843-9E18-AB775FABC034}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>delete</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$S$1:$Y$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1k</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5k</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10k</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50k</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100k</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200k</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$S$3:$Y$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>186</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-447B-F843-9E18-AB775FABC034}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>replace</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$S$1:$Y$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1k</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5k</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10k</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50k</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100k</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200k</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$S$4:$Y$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>370</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-447B-F843-9E18-AB775FABC034}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>upsert</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$S$1:$Y$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1k</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5k</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10k</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50k</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100k</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200k</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$S$5:$Y$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>370</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-447B-F843-9E18-AB775FABC034}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1752068000"/>
+        <c:axId val="1752070192"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1752068000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1752070192"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1752070192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1752068000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3193,6 +3876,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3697,6 +4420,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4268,6 +5494,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BCF2183-2DDC-554E-8748-F355F89AE67C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4573,10 +5835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39F99E4-66C7-D54E-86DA-6485142FBA5F}">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X90" sqref="X90"/>
+    <sheetView tabSelected="1" topLeftCell="Y6" workbookViewId="0">
+      <selection activeCell="AL6" sqref="AL6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4584,7 +5846,7 @@
     <col min="1" max="1" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4621,8 +5883,38 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
+      <c r="O1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W1" t="s">
+        <v>47</v>
+      </c>
+      <c r="X1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4659,8 +5951,38 @@
       <c r="L2">
         <v>7</v>
       </c>
+      <c r="O2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2">
+        <v>7</v>
+      </c>
+      <c r="R2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S2">
+        <v>7</v>
+      </c>
+      <c r="T2">
+        <v>8</v>
+      </c>
+      <c r="U2">
+        <v>10</v>
+      </c>
+      <c r="V2">
+        <v>24</v>
+      </c>
+      <c r="W2">
+        <v>49</v>
+      </c>
+      <c r="X2">
+        <v>99</v>
+      </c>
+      <c r="Y2">
+        <v>186</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -4697,8 +6019,38 @@
       <c r="L3">
         <v>8</v>
       </c>
+      <c r="O3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3">
+        <v>8</v>
+      </c>
+      <c r="R3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S3">
+        <v>7</v>
+      </c>
+      <c r="T3">
+        <v>8</v>
+      </c>
+      <c r="U3">
+        <v>10</v>
+      </c>
+      <c r="V3">
+        <v>24</v>
+      </c>
+      <c r="W3">
+        <v>49</v>
+      </c>
+      <c r="X3">
+        <v>99</v>
+      </c>
+      <c r="Y3">
+        <v>186</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -4735,8 +6087,38 @@
       <c r="L4">
         <v>10</v>
       </c>
+      <c r="O4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4">
+        <v>10</v>
+      </c>
+      <c r="R4" t="s">
+        <v>52</v>
+      </c>
+      <c r="S4">
+        <v>13</v>
+      </c>
+      <c r="T4">
+        <v>14</v>
+      </c>
+      <c r="U4">
+        <v>19</v>
+      </c>
+      <c r="V4">
+        <v>46</v>
+      </c>
+      <c r="W4">
+        <v>97</v>
+      </c>
+      <c r="X4">
+        <v>197</v>
+      </c>
+      <c r="Y4">
+        <v>370</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -4773,8 +6155,38 @@
       <c r="L5">
         <v>24</v>
       </c>
+      <c r="O5" t="s">
+        <v>15</v>
+      </c>
+      <c r="P5">
+        <v>24</v>
+      </c>
+      <c r="R5" t="s">
+        <v>53</v>
+      </c>
+      <c r="S5">
+        <v>13</v>
+      </c>
+      <c r="T5">
+        <v>14</v>
+      </c>
+      <c r="U5">
+        <v>19</v>
+      </c>
+      <c r="V5">
+        <v>46</v>
+      </c>
+      <c r="W5">
+        <v>97</v>
+      </c>
+      <c r="X5">
+        <v>197</v>
+      </c>
+      <c r="Y5">
+        <v>370</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -4811,8 +6223,14 @@
       <c r="L6">
         <v>49</v>
       </c>
+      <c r="O6" t="s">
+        <v>16</v>
+      </c>
+      <c r="P6">
+        <v>49</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -4849,8 +6267,14 @@
       <c r="L7">
         <v>99</v>
       </c>
+      <c r="O7" t="s">
+        <v>17</v>
+      </c>
+      <c r="P7">
+        <v>99</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -4887,8 +6311,14 @@
       <c r="L8">
         <v>186</v>
       </c>
+      <c r="O8" t="s">
+        <v>18</v>
+      </c>
+      <c r="P8">
+        <v>186</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -4925,8 +6355,14 @@
       <c r="L9">
         <v>7</v>
       </c>
+      <c r="O9" t="s">
+        <v>19</v>
+      </c>
+      <c r="P9">
+        <v>7</v>
+      </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -4963,8 +6399,14 @@
       <c r="L10">
         <v>8</v>
       </c>
+      <c r="O10" t="s">
+        <v>20</v>
+      </c>
+      <c r="P10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -5001,8 +6443,14 @@
       <c r="L11">
         <v>10</v>
       </c>
+      <c r="O11" t="s">
+        <v>21</v>
+      </c>
+      <c r="P11">
+        <v>10</v>
+      </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -5039,8 +6487,14 @@
       <c r="L12">
         <v>24</v>
       </c>
+      <c r="O12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P12">
+        <v>24</v>
+      </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -5077,8 +6531,14 @@
       <c r="L13">
         <v>49</v>
       </c>
+      <c r="O13" t="s">
+        <v>23</v>
+      </c>
+      <c r="P13">
+        <v>49</v>
+      </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -5115,8 +6575,14 @@
       <c r="L14">
         <v>99</v>
       </c>
+      <c r="O14" t="s">
+        <v>24</v>
+      </c>
+      <c r="P14">
+        <v>99</v>
+      </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -5153,8 +6619,14 @@
       <c r="L15">
         <v>186</v>
       </c>
+      <c r="O15" t="s">
+        <v>25</v>
+      </c>
+      <c r="P15">
+        <v>186</v>
+      </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -5191,8 +6663,14 @@
       <c r="L16">
         <v>13</v>
       </c>
+      <c r="O16" t="s">
+        <v>26</v>
+      </c>
+      <c r="P16">
+        <v>13</v>
+      </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -5229,8 +6707,14 @@
       <c r="L17">
         <v>14</v>
       </c>
+      <c r="O17" t="s">
+        <v>27</v>
+      </c>
+      <c r="P17">
+        <v>14</v>
+      </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -5267,8 +6751,14 @@
       <c r="L18">
         <v>19</v>
       </c>
+      <c r="O18" t="s">
+        <v>28</v>
+      </c>
+      <c r="P18">
+        <v>19</v>
+      </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -5305,8 +6795,14 @@
       <c r="L19">
         <v>46</v>
       </c>
+      <c r="O19" t="s">
+        <v>29</v>
+      </c>
+      <c r="P19">
+        <v>46</v>
+      </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -5343,8 +6839,14 @@
       <c r="L20">
         <v>97</v>
       </c>
+      <c r="O20" t="s">
+        <v>30</v>
+      </c>
+      <c r="P20">
+        <v>97</v>
+      </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -5381,8 +6883,14 @@
       <c r="L21">
         <v>197</v>
       </c>
+      <c r="O21" t="s">
+        <v>31</v>
+      </c>
+      <c r="P21">
+        <v>197</v>
+      </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -5419,8 +6927,14 @@
       <c r="L22">
         <v>370</v>
       </c>
+      <c r="O22" t="s">
+        <v>32</v>
+      </c>
+      <c r="P22">
+        <v>370</v>
+      </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -5457,8 +6971,14 @@
       <c r="L23">
         <v>13</v>
       </c>
+      <c r="O23" t="s">
+        <v>33</v>
+      </c>
+      <c r="P23">
+        <v>13</v>
+      </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -5495,8 +7015,14 @@
       <c r="L24">
         <v>14</v>
       </c>
+      <c r="O24" t="s">
+        <v>34</v>
+      </c>
+      <c r="P24">
+        <v>14</v>
+      </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -5533,8 +7059,14 @@
       <c r="L25">
         <v>19</v>
       </c>
+      <c r="O25" t="s">
+        <v>35</v>
+      </c>
+      <c r="P25">
+        <v>19</v>
+      </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -5571,8 +7103,14 @@
       <c r="L26">
         <v>46</v>
       </c>
+      <c r="O26" t="s">
+        <v>36</v>
+      </c>
+      <c r="P26">
+        <v>46</v>
+      </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -5609,8 +7147,14 @@
       <c r="L27">
         <v>97</v>
       </c>
+      <c r="O27" t="s">
+        <v>37</v>
+      </c>
+      <c r="P27">
+        <v>97</v>
+      </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -5647,8 +7191,14 @@
       <c r="L28">
         <v>197</v>
       </c>
+      <c r="O28" t="s">
+        <v>38</v>
+      </c>
+      <c r="P28">
+        <v>197</v>
+      </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -5683,6 +7233,12 @@
         <v>370</v>
       </c>
       <c r="L29">
+        <v>370</v>
+      </c>
+      <c r="O29" t="s">
+        <v>39</v>
+      </c>
+      <c r="P29">
         <v>370</v>
       </c>
     </row>

</xml_diff>